<commit_message>
Add: Final evaluation and readme
</commit_message>
<xml_diff>
--- a/data/fruit_data_clean.xlsx
+++ b/data/fruit_data_clean.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E195"/>
+  <dimension ref="A1:E197"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1193,149 +1193,149 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>apple</t>
+          <t>grape</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Purple</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Tiny</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>72.03624304100931</v>
+        <v>10.90219764355227</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>apple</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Creamy White</t>
+          <t>Green</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>78.37478669849315</v>
+        <v>72.03624304100931</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>grape</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Black</t>
+          <t>Creamy White</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Small</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>4.651554367790371</v>
+        <v>78.37478669849315</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>apple</t>
+          <t>grape</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Black</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Small</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>114.8459420846269</v>
+        <v>4.651554367790371</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>grape</t>
+          <t>apple</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Red</t>
+          <t>Green</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Tiny</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>7.668747038278322</v>
+        <v>114.8459420846269</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>apple</t>
+          <t>grape</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Red</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Small</t>
+          <t>Tiny</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>92.57893394687147</v>
+        <v>7.668747038278322</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>grape</t>
+          <t>apple</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1345,20 +1345,20 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Small</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>5.822352898673</v>
+        <v>92.57893394687147</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>grape</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1368,16 +1368,16 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>39.07244747617934</v>
+        <v>5.822352898673</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
@@ -1386,7 +1386,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Pale Yellow</t>
+          <t>Green</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1395,104 +1395,104 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>94.36781460525788</v>
+        <v>39.07244747617934</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>grape</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Black</t>
+          <t>Pale Yellow</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Tiny</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>6.646753328493755</v>
+        <v>94.36781460525788</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>grape</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Yellow</t>
+          <t>Black</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Tiny</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>116.380542680262</v>
+        <v>6.646753328493755</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>grape</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Yellow</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Tiny</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>4.824470755007685</v>
+        <v>116.380542680262</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>apple</t>
+          <t>grape</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Red</t>
+          <t>Green</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Tiny</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>108.0344695638916</v>
+        <v>4.824470755007685</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
@@ -1506,16 +1506,16 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Small</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>92.03583555146749</v>
+        <v>108.0344695638916</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
@@ -1524,7 +1524,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Red</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1533,21 +1533,21 @@
         </is>
       </c>
       <c r="E48" t="n">
-        <v>81.29824150939457</v>
+        <v>92.03583555146749</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>apple</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Creamy White</t>
+          <t>Green</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1556,81 +1556,81 @@
         </is>
       </c>
       <c r="E49" t="n">
-        <v>32.32644964238034</v>
+        <v>81.29824150939457</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>grape</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Red</t>
+          <t>Creamy White</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Tiny</t>
+          <t>Small</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>6.366469143736201</v>
+        <v>32.32644964238034</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>grape</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Pale Yellow</t>
+          <t>Red</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Tiny</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>101.649727964565</v>
+        <v>6.366469143736201</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>grape</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Yellow</t>
+          <t>Pale Yellow</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E52" t="n">
-        <v>6.452329858757221</v>
+        <v>101.649727964565</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
@@ -1639,90 +1639,90 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Black</t>
+          <t>Yellow</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Small</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>6.646753328493755</v>
+        <v>6.452329858757221</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>apple</t>
+          <t>grape</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Yellow</t>
+          <t>Black</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Small</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>68.72025424364693</v>
+        <v>6.646753328493755</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>apple</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Creamy White</t>
+          <t>Yellow</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Small</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E55" t="n">
-        <v>116.380542680262</v>
+        <v>68.72025424364693</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>apple</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Red</t>
+          <t>Creamy White</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Small</t>
         </is>
       </c>
       <c r="E56" t="n">
-        <v>50.57733667875135</v>
+        <v>116.380542680262</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
@@ -1731,7 +1731,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Red</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1740,21 +1740,21 @@
         </is>
       </c>
       <c r="E57" t="n">
-        <v>85.24782703146265</v>
+        <v>50.57733667875135</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>apple</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Creamy White</t>
+          <t>Green</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -1763,35 +1763,35 @@
         </is>
       </c>
       <c r="E58" t="n">
-        <v>101.649727964565</v>
+        <v>85.24782703146265</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>grape</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Red</t>
+          <t>Creamy White</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Tiny</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E59" t="n">
-        <v>6.215846474504573</v>
+        <v>101.649727964565</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
@@ -1800,7 +1800,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Purple</t>
+          <t>Red</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1809,12 +1809,12 @@
         </is>
       </c>
       <c r="E60" t="n">
-        <v>9.774545560187402</v>
+        <v>6.215846474504573</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
@@ -1823,25 +1823,25 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Yellow</t>
+          <t>Purple</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Tiny</t>
         </is>
       </c>
       <c r="E61" t="n">
-        <v>4.309717913320138</v>
+        <v>9.774545560187402</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>grape</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -1851,16 +1851,16 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Small</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>107.7779183618232</v>
+        <v>4.309717913320138</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
@@ -1869,21 +1869,21 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Yellow</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Small</t>
         </is>
       </c>
       <c r="E63" t="n">
-        <v>78.37478669849315</v>
+        <v>107.7779183618232</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
@@ -1892,21 +1892,21 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Yellow</t>
+          <t>Green</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>32.32644964238034</v>
+        <v>78.37478669849315</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
@@ -1915,53 +1915,53 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Yellow</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="E65" t="n">
-        <v>109.3762728729673</v>
+        <v>32.32644964238034</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>apple</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Red</t>
+          <t>Green</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Small</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E66" t="n">
-        <v>92.59265388351021</v>
+        <v>109.3762728729673</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>grape</t>
+          <t>apple</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Black</t>
+          <t>Red</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -1970,21 +1970,21 @@
         </is>
       </c>
       <c r="E67" t="n">
-        <v>4.651554367790371</v>
+        <v>92.59265388351021</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>apple</t>
+          <t>grape</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Pink</t>
+          <t>Black</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -1993,44 +1993,44 @@
         </is>
       </c>
       <c r="E68" t="n">
-        <v>96.04021591528162</v>
+        <v>4.651554367790371</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>apple</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Creamy White</t>
+          <t>Pink</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Small</t>
         </is>
       </c>
       <c r="E69" t="n">
-        <v>89.71911557187848</v>
+        <v>96.04021591528162</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>apple</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Creamy White</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2039,12 +2039,12 @@
         </is>
       </c>
       <c r="E70" t="n">
-        <v>118.1736162455458</v>
+        <v>89.71911557187848</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
@@ -2053,67 +2053,67 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Pink</t>
+          <t>Green</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="E71" t="n">
-        <v>73.27469354853721</v>
+        <v>118.1736162455458</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>grape</t>
+          <t>apple</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Red</t>
+          <t>Pink</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Small</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E72" t="n">
-        <v>7.668747038278322</v>
+        <v>73.27469354853721</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>apple</t>
+          <t>grape</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Red</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Small</t>
         </is>
       </c>
       <c r="E73" t="n">
-        <v>72.03624304100931</v>
+        <v>7.668747038278322</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
@@ -2122,7 +2122,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Yellow</t>
+          <t>Green</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -2131,67 +2131,67 @@
         </is>
       </c>
       <c r="E74" t="n">
-        <v>92.57893394687147</v>
+        <v>72.03624304100931</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>grape</t>
+          <t>apple</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Yellow</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Small</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E75" t="n">
-        <v>9.269920663824788</v>
+        <v>92.57893394687147</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>grape</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Yellow</t>
+          <t>Green</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Small</t>
         </is>
       </c>
       <c r="E76" t="n">
-        <v>101.649727964565</v>
+        <v>9.269920663824788</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>apple</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Yellow</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -2200,44 +2200,44 @@
         </is>
       </c>
       <c r="E77" t="n">
-        <v>123.068395162833</v>
+        <v>101.649727964565</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>grape</t>
+          <t>apple</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Yellow</t>
+          <t>Green</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Small</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E78" t="n">
-        <v>7.329652827044423</v>
+        <v>123.068395162833</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>apple</t>
+          <t>grape</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Pink</t>
+          <t>Yellow</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -2246,21 +2246,21 @@
         </is>
       </c>
       <c r="E79" t="n">
-        <v>43.28796930186649</v>
+        <v>7.329652827044423</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>grape</t>
+          <t>apple</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Purple</t>
+          <t>Pink</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -2269,35 +2269,35 @@
         </is>
       </c>
       <c r="E80" t="n">
-        <v>8.303384789523257</v>
+        <v>43.28796930186649</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>apple</t>
+          <t>grape</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Yellow</t>
+          <t>Purple</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Small</t>
         </is>
       </c>
       <c r="E81" t="n">
-        <v>106.2719313945375</v>
+        <v>8.303384789523257</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
@@ -2306,25 +2306,25 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Yellow</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E82" t="n">
-        <v>99.18898489065374</v>
+        <v>106.2719313945375</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>grape</t>
+          <t>apple</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -2338,35 +2338,35 @@
         </is>
       </c>
       <c r="E83" t="n">
-        <v>5.822352898673</v>
+        <v>99.18898489065374</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>grape</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Creamy White</t>
+          <t>Green</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Small</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="E84" t="n">
-        <v>45.13167595167246</v>
+        <v>5.822352898673</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
@@ -2375,21 +2375,21 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Creamy White</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Small</t>
         </is>
       </c>
       <c r="E85" t="n">
-        <v>116.374841429252</v>
+        <v>45.13167595167246</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
@@ -2398,53 +2398,53 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Creamy White</t>
+          <t>Green</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Small</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="E86" t="n">
-        <v>32.32644964238034</v>
+        <v>116.374841429252</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>apple</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Red</t>
+          <t>Creamy White</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Small</t>
         </is>
       </c>
       <c r="E87" t="n">
-        <v>118.1736162455458</v>
+        <v>32.32644964238034</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>apple</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Creamy White</t>
+          <t>Red</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -2453,81 +2453,81 @@
         </is>
       </c>
       <c r="E88" t="n">
-        <v>79.90323493698043</v>
+        <v>118.1736162455458</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>apple</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Yellow</t>
+          <t>Creamy White</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="E89" t="n">
-        <v>106.2719313945375</v>
+        <v>79.90323493698043</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>grape</t>
+          <t>apple</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Purple</t>
+          <t>Yellow</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E90" t="n">
-        <v>4.824470755007685</v>
+        <v>106.2719313945375</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>apple</t>
+          <t>grape</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Red</t>
+          <t>Purple</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Small</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="E91" t="n">
-        <v>43.28796930186649</v>
+        <v>4.824470755007685</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
@@ -2536,21 +2536,21 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Pink</t>
+          <t>Red</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Small</t>
         </is>
       </c>
       <c r="E92" t="n">
-        <v>50.57733667875135</v>
+        <v>43.28796930186649</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
@@ -2559,7 +2559,7 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Red</t>
+          <t>Pink</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -2568,12 +2568,12 @@
         </is>
       </c>
       <c r="E93" t="n">
-        <v>92.59265388351021</v>
+        <v>50.57733667875135</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
@@ -2582,7 +2582,7 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Pink</t>
+          <t>Red</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -2591,12 +2591,12 @@
         </is>
       </c>
       <c r="E94" t="n">
-        <v>86.7392400592732</v>
+        <v>92.59265388351021</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
@@ -2605,25 +2605,25 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Yellow</t>
+          <t>Pink</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E95" t="n">
-        <v>25.03832256472326</v>
+        <v>86.7392400592732</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>apple</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -2637,44 +2637,44 @@
         </is>
       </c>
       <c r="E96" t="n">
-        <v>74.61519234331983</v>
+        <v>25.03832256472326</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>apple</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Red</t>
+          <t>Yellow</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Small</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="E97" t="n">
-        <v>106.2719313945375</v>
+        <v>74.61519234331983</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>grape</t>
+          <t>apple</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Yellow</t>
+          <t>Red</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -2683,21 +2683,21 @@
         </is>
       </c>
       <c r="E98" t="n">
-        <v>5.822352898673</v>
+        <v>106.2719313945375</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>apple</t>
+          <t>grape</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Yellow</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -2706,16 +2706,16 @@
         </is>
       </c>
       <c r="E99" t="n">
-        <v>123.068395162833</v>
+        <v>5.822352898673</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>apple</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -2725,20 +2725,20 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Small</t>
         </is>
       </c>
       <c r="E100" t="n">
-        <v>56.05648981655342</v>
+        <v>123.068395162833</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>apple</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -2748,39 +2748,39 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="E101" t="n">
-        <v>130.7218665281646</v>
+        <v>56.05648981655342</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>apple</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Yellow</t>
+          <t>Green</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E102" t="n">
-        <v>54.83180911374895</v>
+        <v>130.7218665281646</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
@@ -2794,39 +2794,39 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="E103" t="n">
-        <v>116.380542680262</v>
+        <v>54.83180911374895</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>grape</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Black</t>
+          <t>Yellow</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Small</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E104" t="n">
-        <v>6.461906344196531</v>
+        <v>116.380542680262</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
@@ -2840,43 +2840,43 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Small</t>
         </is>
       </c>
       <c r="E105" t="n">
-        <v>6.807726509609703</v>
+        <v>6.461906344196531</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>grape</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Black</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="E106" t="n">
-        <v>70.31401278637242</v>
+        <v>6.807726509609703</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>grape</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -2886,39 +2886,39 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>Small</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E107" t="n">
-        <v>6.461906344196531</v>
+        <v>70.31401278637242</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>grape</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>Yellow</t>
+          <t>Green</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Small</t>
         </is>
       </c>
       <c r="E108" t="n">
-        <v>56.05648981655342</v>
+        <v>6.461906344196531</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
@@ -2927,48 +2927,48 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>Pale Yellow</t>
+          <t>Yellow</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="E109" t="n">
-        <v>107.7779183618232</v>
+        <v>56.05648981655342</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>apple</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>Yellow</t>
+          <t>Pale Yellow</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E110" t="n">
-        <v>85.24782703146265</v>
+        <v>107.7779183618232</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>grape</t>
+          <t>apple</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -2978,25 +2978,25 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>Small</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="E111" t="n">
-        <v>6.461906344196531</v>
+        <v>85.24782703146265</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>grape</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Creamy White</t>
+          <t>Yellow</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -3005,81 +3005,81 @@
         </is>
       </c>
       <c r="E112" t="n">
-        <v>94.43263330047935</v>
+        <v>6.461906344196531</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>apple</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Red</t>
+          <t>Creamy White</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Small</t>
         </is>
       </c>
       <c r="E113" t="n">
-        <v>68.72025424364693</v>
+        <v>94.43263330047935</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>apple</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Red</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="E114" t="n">
-        <v>93.43820611693542</v>
+        <v>68.72025424364693</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>apple</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Red</t>
+          <t>Green</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E115" t="n">
-        <v>85.18897978616607</v>
+        <v>93.43820611693542</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
@@ -3088,25 +3088,25 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Yellow</t>
+          <t>Red</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="E116" t="n">
-        <v>92.57893394687147</v>
+        <v>85.18897978616607</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>apple</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -3120,12 +3120,12 @@
         </is>
       </c>
       <c r="E117" t="n">
-        <v>94.36781460525788</v>
+        <v>92.57893394687147</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
@@ -3134,21 +3134,21 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Pale Yellow</t>
+          <t>Yellow</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E118" t="n">
-        <v>57.49857482332844</v>
+        <v>94.36781460525788</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
@@ -3157,12 +3157,12 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Creamy White</t>
+          <t>Pale Yellow</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>Small</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="E119" t="n">
@@ -3171,53 +3171,53 @@
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>grape</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Creamy White</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>Tiny</t>
+          <t>Small</t>
         </is>
       </c>
       <c r="E120" t="n">
-        <v>8.303384789523257</v>
+        <v>57.49857482332844</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>grape</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>Yellow</t>
+          <t>Green</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Tiny</t>
         </is>
       </c>
       <c r="E121" t="n">
-        <v>70.31401278637242</v>
+        <v>8.303384789523257</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
@@ -3231,62 +3231,62 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E122" t="n">
-        <v>26.52458652516574</v>
+        <v>70.31401278637242</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>apple</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>Red</t>
+          <t>Yellow</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="E123" t="n">
-        <v>68.72025424364693</v>
+        <v>26.52458652516574</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>grape</t>
+          <t>apple</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Purple</t>
+          <t>Red</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>Small</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E124" t="n">
-        <v>6.366469143736201</v>
+        <v>68.72025424364693</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
@@ -3304,21 +3304,21 @@
         </is>
       </c>
       <c r="E125" t="n">
-        <v>9.774545560187402</v>
+        <v>6.366469143736201</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>apple</t>
+          <t>grape</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Purple</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
@@ -3327,62 +3327,62 @@
         </is>
       </c>
       <c r="E126" t="n">
-        <v>106.2719313945375</v>
+        <v>9.774545560187402</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>apple</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>Yellow</t>
+          <t>Green</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Small</t>
         </is>
       </c>
       <c r="E127" t="n">
-        <v>56.05648981655342</v>
+        <v>106.2719313945375</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>apple</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Yellow</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E128" t="n">
-        <v>92.59265388351021</v>
+        <v>56.05648981655342</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>apple</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -3392,16 +3392,16 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="E129" t="n">
-        <v>39.07244747617934</v>
+        <v>92.59265388351021</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B130" t="inlineStr">
         <is>
@@ -3415,48 +3415,48 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>Small</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E130" t="n">
-        <v>46.14579018758998</v>
+        <v>39.07244747617934</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>apple</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>Red</t>
+          <t>Green</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Small</t>
         </is>
       </c>
       <c r="E131" t="n">
-        <v>50.57733667875135</v>
+        <v>46.14579018758998</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>apple</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>Yellow</t>
+          <t>Red</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
@@ -3465,12 +3465,12 @@
         </is>
       </c>
       <c r="E132" t="n">
-        <v>77.12120021499526</v>
+        <v>50.57733667875135</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B133" t="inlineStr">
         <is>
@@ -3479,7 +3479,7 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Yellow</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
@@ -3488,16 +3488,16 @@
         </is>
       </c>
       <c r="E133" t="n">
-        <v>94.36781460525788</v>
+        <v>77.12120021499526</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>grape</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -3507,16 +3507,16 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E134" t="n">
-        <v>6.366469143736201</v>
+        <v>94.36781460525788</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B135" t="inlineStr">
         <is>
@@ -3525,7 +3525,7 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>Red</t>
+          <t>Green</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
@@ -3534,12 +3534,12 @@
         </is>
       </c>
       <c r="E135" t="n">
-        <v>7.210973735368247</v>
+        <v>6.366469143736201</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B136" t="inlineStr">
         <is>
@@ -3548,21 +3548,21 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Red</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>Small</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="E136" t="n">
-        <v>9.909564657481351</v>
+        <v>7.210973735368247</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B137" t="inlineStr">
         <is>
@@ -3571,25 +3571,25 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>Yellow</t>
+          <t>Green</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>Tiny</t>
+          <t>Small</t>
         </is>
       </c>
       <c r="E137" t="n">
-        <v>9.456228491200928</v>
+        <v>10.90219764355227</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>grape</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -3599,62 +3599,62 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Small</t>
         </is>
       </c>
       <c r="E138" t="n">
-        <v>26.52458652516574</v>
+        <v>9.909564657481351</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>grape</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>Creamy White</t>
+          <t>Yellow</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Tiny</t>
         </is>
       </c>
       <c r="E139" t="n">
-        <v>57.49857482332844</v>
+        <v>9.456228491200928</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>grape</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>Purple</t>
+          <t>Green</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>Small</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E140" t="n">
-        <v>9.456228491200928</v>
+        <v>26.52458652516574</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B141" t="inlineStr">
         <is>
@@ -3663,7 +3663,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Creamy White</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
@@ -3672,12 +3672,12 @@
         </is>
       </c>
       <c r="E141" t="n">
-        <v>94.43263330047935</v>
+        <v>57.49857482332844</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B142" t="inlineStr">
         <is>
@@ -3686,30 +3686,30 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>Black</t>
+          <t>Purple</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>Tiny</t>
+          <t>Small</t>
         </is>
       </c>
       <c r="E142" t="n">
-        <v>6.461906344196531</v>
+        <v>9.456228491200928</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>grape</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>Black</t>
+          <t>Green</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
@@ -3718,12 +3718,12 @@
         </is>
       </c>
       <c r="E143" t="n">
-        <v>5.717561341186324</v>
+        <v>94.43263330047935</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B144" t="inlineStr">
         <is>
@@ -3732,21 +3732,21 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>Yellow</t>
+          <t>Black</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Tiny</t>
         </is>
       </c>
       <c r="E144" t="n">
-        <v>4.824470755007685</v>
+        <v>6.461906344196531</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B145" t="inlineStr">
         <is>
@@ -3755,21 +3755,21 @@
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>Yellow</t>
+          <t>Black</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>Small</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="E145" t="n">
-        <v>5.371310191898408</v>
+        <v>5.717561341186324</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B146" t="inlineStr">
         <is>
@@ -3783,39 +3783,39 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>Small</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="E146" t="n">
-        <v>5.371310191898408</v>
+        <v>4.824470755007685</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="n">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>apple</t>
+          <t>grape</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>Pink</t>
+          <t>Yellow</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Small</t>
         </is>
       </c>
       <c r="E147" t="n">
-        <v>130.7218665281646</v>
+        <v>5.371310191898408</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="n">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B148" t="inlineStr">
         <is>
@@ -3829,16 +3829,16 @@
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>Tiny</t>
+          <t>Small</t>
         </is>
       </c>
       <c r="E148" t="n">
-        <v>9.456228491200928</v>
+        <v>5.371310191898408</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="n">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B149" t="inlineStr">
         <is>
@@ -3847,7 +3847,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Pink</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
@@ -3856,16 +3856,16 @@
         </is>
       </c>
       <c r="E149" t="n">
-        <v>43.28796930186649</v>
+        <v>130.7218665281646</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="1" t="n">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>apple</t>
+          <t>grape</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
@@ -3875,39 +3875,39 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Tiny</t>
         </is>
       </c>
       <c r="E150" t="n">
-        <v>96.38009167486044</v>
+        <v>9.456228491200928</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="n">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>apple</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>Creamy White</t>
+          <t>Green</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>Small</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E151" t="n">
-        <v>78.37478669849315</v>
+        <v>43.28796930186649</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="n">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B152" t="inlineStr">
         <is>
@@ -3916,7 +3916,7 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>Pink</t>
+          <t>Yellow</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
@@ -3925,173 +3925,173 @@
         </is>
       </c>
       <c r="E152" t="n">
-        <v>123.068395162833</v>
+        <v>96.38009167486044</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="1" t="n">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>grape</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>Black</t>
+          <t>Creamy White</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Small</t>
         </is>
       </c>
       <c r="E153" t="n">
-        <v>6.461906344196531</v>
+        <v>78.37478669849315</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="n">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>grape</t>
+          <t>apple</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Pink</t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E154" t="n">
-        <v>6.646753328493755</v>
+        <v>123.068395162833</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="1" t="n">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>grape</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>Yellow</t>
+          <t>Black</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="E155" t="n">
-        <v>78.37478669849315</v>
+        <v>6.461906344196531</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="1" t="n">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>grape</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>Yellow</t>
+          <t>Green</t>
         </is>
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="E156" t="n">
-        <v>57.22769751652829</v>
+        <v>6.646753328493755</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="1" t="n">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>grape</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>Red</t>
+          <t>Yellow</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E157" t="n">
-        <v>7.668747038278322</v>
+        <v>78.37478669849315</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="1" t="n">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>apple</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>Pink</t>
+          <t>Yellow</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>Small</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E158" t="n">
-        <v>108.0344695638916</v>
+        <v>57.22769751652829</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="n">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>apple</t>
+          <t>grape</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>Yellow</t>
+          <t>Red</t>
         </is>
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="E159" t="n">
-        <v>123.068395162833</v>
+        <v>7.668747038278322</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="n">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B160" t="inlineStr">
         <is>
@@ -4100,21 +4100,21 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Pink</t>
         </is>
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Small</t>
         </is>
       </c>
       <c r="E160" t="n">
-        <v>96.04021591528162</v>
+        <v>108.0344695638916</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="n">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B161" t="inlineStr">
         <is>
@@ -4123,21 +4123,21 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>Red</t>
+          <t>Yellow</t>
         </is>
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>Small</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E161" t="n">
-        <v>108.0344695638916</v>
+        <v>123.068395162833</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="n">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B162" t="inlineStr">
         <is>
@@ -4155,12 +4155,12 @@
         </is>
       </c>
       <c r="E162" t="n">
-        <v>68.72025424364693</v>
+        <v>96.04021591528162</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="n">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B163" t="inlineStr">
         <is>
@@ -4169,7 +4169,7 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>Pink</t>
+          <t>Red</t>
         </is>
       </c>
       <c r="D163" t="inlineStr">
@@ -4178,12 +4178,12 @@
         </is>
       </c>
       <c r="E163" t="n">
-        <v>80.97637017991676</v>
+        <v>108.0344695638916</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="n">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B164" t="inlineStr">
         <is>
@@ -4192,136 +4192,136 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>Pink</t>
+          <t>Green</t>
         </is>
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E164" t="n">
-        <v>85.18897978616607</v>
+        <v>68.72025424364693</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="n">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>apple</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>Creamy White</t>
+          <t>Pink</t>
         </is>
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Small</t>
         </is>
       </c>
       <c r="E165" t="n">
-        <v>77.12120021499526</v>
+        <v>80.97637017991676</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="1" t="n">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>grape</t>
+          <t>apple</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>Yellow</t>
+          <t>Pink</t>
         </is>
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>Tiny</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="E166" t="n">
-        <v>5.717561341186324</v>
+        <v>85.18897978616607</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="1" t="n">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>apple</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>Pink</t>
+          <t>Creamy White</t>
         </is>
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="E167" t="n">
-        <v>68.72025424364693</v>
+        <v>77.12120021499526</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="n">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>apple</t>
+          <t>grape</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Yellow</t>
         </is>
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>Small</t>
+          <t>Tiny</t>
         </is>
       </c>
       <c r="E168" t="n">
-        <v>137.927572006952</v>
+        <v>5.717561341186324</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="n">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>grape</t>
+          <t>apple</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>Yellow</t>
+          <t>Pink</t>
         </is>
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>Tiny</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E169" t="n">
-        <v>6.3704802406948</v>
+        <v>68.72025424364693</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="n">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B170" t="inlineStr">
         <is>
@@ -4330,67 +4330,67 @@
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>Pink</t>
+          <t>Green</t>
         </is>
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Small</t>
         </is>
       </c>
       <c r="E170" t="n">
-        <v>118.1736162455458</v>
+        <v>137.927572006952</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="n">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>grape</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Yellow</t>
         </is>
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>Small</t>
+          <t>Tiny</t>
         </is>
       </c>
       <c r="E171" t="n">
-        <v>116.380542680262</v>
+        <v>6.3704802406948</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="1" t="n">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>apple</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Pink</t>
         </is>
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="E172" t="n">
-        <v>46.14579018758998</v>
+        <v>118.1736162455458</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="n">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B173" t="inlineStr">
         <is>
@@ -4408,21 +4408,21 @@
         </is>
       </c>
       <c r="E173" t="n">
-        <v>98.50786925613157</v>
+        <v>116.380542680262</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="n">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>apple</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>Red</t>
+          <t>Green</t>
         </is>
       </c>
       <c r="D174" t="inlineStr">
@@ -4431,21 +4431,21 @@
         </is>
       </c>
       <c r="E174" t="n">
-        <v>25.03832256472326</v>
+        <v>46.14579018758998</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="1" t="n">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>apple</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>Yellow</t>
+          <t>Green</t>
         </is>
       </c>
       <c r="D175" t="inlineStr">
@@ -4454,35 +4454,35 @@
         </is>
       </c>
       <c r="E175" t="n">
-        <v>96.38009167486044</v>
+        <v>98.50786925613157</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="n">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>apple</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>Creamy White</t>
+          <t>Red</t>
         </is>
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>Small</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E176" t="n">
-        <v>32.32644964238034</v>
+        <v>25.03832256472326</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="n">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B177" t="inlineStr">
         <is>
@@ -4491,12 +4491,12 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>Red</t>
+          <t>Yellow</t>
         </is>
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Small</t>
         </is>
       </c>
       <c r="E177" t="n">
@@ -4505,16 +4505,16 @@
     </row>
     <row r="178">
       <c r="A178" s="1" t="n">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>apple</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>Red</t>
+          <t>Creamy White</t>
         </is>
       </c>
       <c r="D178" t="inlineStr">
@@ -4523,62 +4523,62 @@
         </is>
       </c>
       <c r="E178" t="n">
-        <v>92.03583555146749</v>
+        <v>32.32644964238034</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="n">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>apple</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Red</t>
         </is>
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E179" t="n">
-        <v>109.3762728729673</v>
+        <v>96.38009167486044</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="1" t="n">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>apple</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Red</t>
         </is>
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Small</t>
         </is>
       </c>
       <c r="E180" t="n">
-        <v>57.49857482332844</v>
+        <v>92.03583555146749</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="1" t="n">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>grape</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
@@ -4588,39 +4588,39 @@
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t>Tiny</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="E181" t="n">
-        <v>6.807726509609703</v>
+        <v>109.3762728729673</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="1" t="n">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>grape</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>Red</t>
+          <t>Green</t>
         </is>
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t>Tiny</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E182" t="n">
-        <v>4.651554367790371</v>
+        <v>57.49857482332844</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="1" t="n">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B183" t="inlineStr">
         <is>
@@ -4629,7 +4629,7 @@
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>Purple</t>
+          <t>Green</t>
         </is>
       </c>
       <c r="D183" t="inlineStr">
@@ -4638,58 +4638,58 @@
         </is>
       </c>
       <c r="E183" t="n">
-        <v>9.856588663715842</v>
+        <v>6.807726509609703</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="1" t="n">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>grape</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>Pale Yellow</t>
+          <t>Red</t>
         </is>
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Tiny</t>
         </is>
       </c>
       <c r="E184" t="n">
-        <v>106.1173684521128</v>
+        <v>4.651554367790371</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="1" t="n">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>grape</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>Creamy White</t>
+          <t>Purple</t>
         </is>
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>Small</t>
+          <t>Tiny</t>
         </is>
       </c>
       <c r="E185" t="n">
-        <v>116.380542680262</v>
+        <v>9.856588663715842</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="1" t="n">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B186" t="inlineStr">
         <is>
@@ -4703,48 +4703,48 @@
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E186" t="n">
-        <v>116.374841429252</v>
+        <v>106.1173684521128</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="1" t="n">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>grape</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>Black</t>
+          <t>Creamy White</t>
         </is>
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Small</t>
         </is>
       </c>
       <c r="E187" t="n">
-        <v>6.215846474504573</v>
+        <v>116.380542680262</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="1" t="n">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>grape</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Pale Yellow</t>
         </is>
       </c>
       <c r="D188" t="inlineStr">
@@ -4753,35 +4753,35 @@
         </is>
       </c>
       <c r="E188" t="n">
-        <v>10.90219764355227</v>
+        <v>116.374841429252</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="1" t="n">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>grape</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Black</t>
         </is>
       </c>
       <c r="D189" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="E189" t="n">
-        <v>46.14579018758998</v>
+        <v>6.215846474504573</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="1" t="n">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B190" t="inlineStr">
         <is>
@@ -4795,62 +4795,62 @@
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>Small</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="E190" t="n">
-        <v>4.309717913320138</v>
+        <v>10.90219764355227</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="n">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>grape</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>Purple</t>
+          <t>Green</t>
         </is>
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>Small</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E191" t="n">
-        <v>9.774545560187402</v>
+        <v>46.14579018758998</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="1" t="n">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>grape</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>Pale Yellow</t>
+          <t>Green</t>
         </is>
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t>Large</t>
+          <t>Small</t>
         </is>
       </c>
       <c r="E192" t="n">
-        <v>39.01296159006213</v>
+        <v>4.309717913320138</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="1" t="n">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B193" t="inlineStr">
         <is>
@@ -4859,7 +4859,7 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>Red</t>
+          <t>Purple</t>
         </is>
       </c>
       <c r="D193" t="inlineStr">
@@ -4868,52 +4868,98 @@
         </is>
       </c>
       <c r="E193" t="n">
-        <v>7.409021364824795</v>
+        <v>9.774545560187402</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="1" t="n">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>grape</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>Red</t>
+          <t>Pale Yellow</t>
         </is>
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Large</t>
         </is>
       </c>
       <c r="E194" t="n">
-        <v>4.651554367790371</v>
+        <v>39.01296159006213</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="1" t="n">
+        <v>197</v>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>grape</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>Small</t>
+        </is>
+      </c>
+      <c r="E195" t="n">
+        <v>7.409021364824795</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="1" t="n">
+        <v>198</v>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>grape</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E196" t="n">
+        <v>4.651554367790371</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="1" t="n">
         <v>199</v>
       </c>
-      <c r="B195" t="inlineStr">
-        <is>
-          <t>grape</t>
-        </is>
-      </c>
-      <c r="C195" t="inlineStr">
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>grape</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
       </c>
-      <c r="D195" t="inlineStr">
+      <c r="D197" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="E195" t="n">
+      <c r="E197" t="n">
         <v>5.937050795675715</v>
       </c>
     </row>

</xml_diff>